<commit_message>
feat: Implement sheet management functionality in admin dashboard
- Added a new SheetsPage component for managing sheet configurations.
- Introduced SheetManager component to handle creation, updating, and deletion of sheets.
- Integrated dynamic form schema generation based on sheet configurations in SubmissionForm.
- Updated AdminDashboard to include a link to manage sheets.
- Enhanced SubmissionsTable to display submissions with corresponding sheet names and dynamic headers.
- Created a new JSON file for initial sheet configurations.
- Added types for SheetConfig and Submission in lib/types.ts.
- Updated package dependencies for better compatibility.
</commit_message>
<xml_diff>
--- a/data/user-submissions.xlsx
+++ b/data/user-submissions.xlsx
@@ -3,7 +3,8 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <workbookPr codeName="ThisWorkbook"/>
   <sheets>
-    <sheet name="Submissions" sheetId="1" r:id="rId1"/>
+    <sheet name="cv-data" sheetId="1" r:id="rId1"/>
+    <sheet name="test" sheetId="2" r:id="rId2"/>
   </sheets>
 </workbook>
 </file>
@@ -397,7 +398,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F3"/>
+  <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -407,64 +408,45 @@
         <v>id</v>
       </c>
       <c r="B1" t="str">
-        <v>name</v>
+        <v>submittedAt</v>
       </c>
       <c r="C1" t="str">
-        <v>email</v>
+        <v>Name</v>
       </c>
       <c r="D1" t="str">
-        <v>phone</v>
-      </c>
-      <c r="E1" t="str">
-        <v>message</v>
-      </c>
-      <c r="F1" t="str">
-        <v>submittedAt</v>
+        <v>Email</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="str">
-        <v>2b93f9fd-b5c8-48f6-81da-506bfd1df367</v>
+        <v>8eaf02eb-5f97-437e-9176-9c1f4dad580e</v>
       </c>
       <c r="B2" t="str">
-        <v>Minal</v>
+        <v>2025-04-26T14:47:40.065Z</v>
       </c>
       <c r="C2" t="str">
+        <v>minal</v>
+      </c>
+      <c r="D2" t="str">
         <v>minal@gmail.com</v>
-      </c>
-      <c r="D2" t="str">
-        <v>2342345325</v>
-      </c>
-      <c r="E2" t="str">
-        <v>werfwe ewr werf</v>
-      </c>
-      <c r="F2" t="str">
-        <v>2025-04-25T08:32:05.287Z</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="str">
-        <v>921f0eaa-ca5e-46c3-9609-e74a12128b22</v>
-      </c>
-      <c r="B3" t="str">
-        <v>minuy</v>
-      </c>
-      <c r="C3" t="str">
-        <v>min@gmail.com</v>
-      </c>
-      <c r="D3" t="str">
-        <v>1124325465</v>
-      </c>
-      <c r="E3" t="str">
-        <v>retgret rty trhytrey</v>
-      </c>
-      <c r="F3" t="str">
-        <v>2025-04-25T16:58:19.147Z</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:F3"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:D2"/>
+  </ignoredErrors>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetData/>
+  <ignoredErrors>
+    <ignoredError numberStoredAsText="1" sqref="A1"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>